<commit_message>
quản lý Học sinh, quản lý lớp học và thêm lọc vào quản lý giáo viên
</commit_message>
<xml_diff>
--- a/src/main/resources/static/asset/DATN/assets/file/file_student.xlsx
+++ b/src/main/resources/static/asset/DATN/assets/file/file_student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26250" windowHeight="12240"/>
+    <workbookView windowWidth="28800" windowHeight="13125"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Mã học sinh</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tên HS</t>
+    <t>Tên HS</t>
   </si>
   <si>
     <t>Birthday</t>
@@ -37,7 +37,7 @@
     <t>Hình</t>
   </si>
   <si>
-    <t>HS0003</t>
+    <t>HS0008</t>
   </si>
   <si>
     <t>Nguyễn Thị Linh Nhi</t>
@@ -46,10 +46,10 @@
     <t>30/6A Hà Thị Khiêm</t>
   </si>
   <si>
-    <t>123.png</t>
-  </si>
-  <si>
-    <t>HS0004</t>
+    <t>13.png</t>
+  </si>
+  <si>
+    <t>HS0009</t>
   </si>
   <si>
     <t>Nguyễn Trần Văn Thuận</t>
@@ -61,10 +61,10 @@
     <t>học sinh chuyển trường</t>
   </si>
   <si>
-    <t>456.png</t>
-  </si>
-  <si>
-    <t>HS0005</t>
+    <t>14.png</t>
+  </si>
+  <si>
+    <t>HS0010</t>
   </si>
   <si>
     <t>Hoàng Tân Đại</t>
@@ -76,13 +76,16 @@
     <t>sắp đi nghĩa vụ</t>
   </si>
   <si>
-    <t>789.png</t>
-  </si>
-  <si>
-    <t>HS0006</t>
+    <t>15.png</t>
+  </si>
+  <si>
+    <t>HS0011</t>
   </si>
   <si>
     <t>Trương Hoàng Giang</t>
+  </si>
+  <si>
+    <t>16.png</t>
   </si>
 </sst>
 </file>
@@ -90,13 +93,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +108,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -126,24 +131,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,46 +223,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,19 +269,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +413,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,163 +453,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -554,15 +580,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -572,138 +598,144 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,7 +1060,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -1042,25 +1074,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1071,7 +1103,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>37238</v>
       </c>
       <c r="D2" t="b">
@@ -1080,7 +1112,7 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1091,7 +1123,7 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>37165</v>
       </c>
       <c r="D3" t="b">
@@ -1103,7 +1135,7 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1114,7 +1146,7 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>37101</v>
       </c>
       <c r="D4" t="b">
@@ -1126,7 +1158,7 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1137,7 +1169,7 @@
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>37101</v>
       </c>
       <c r="D5" t="b">
@@ -1146,9 +1178,8 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="F5"/>
-      <c r="G5" t="s">
-        <v>20</v>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chỉnh sửa validation và thêm hình ảnh
</commit_message>
<xml_diff>
--- a/src/main/resources/static/asset/DATN/assets/file/file_student.xlsx
+++ b/src/main/resources/static/asset/DATN/assets/file/file_student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13125"/>
+    <workbookView windowWidth="20490" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Mã học sinh</t>
   </si>
@@ -37,7 +37,10 @@
     <t>Hình</t>
   </si>
   <si>
-    <t>HS0008</t>
+    <t>SDT phụ huynh</t>
+  </si>
+  <si>
+    <t>HS0050</t>
   </si>
   <si>
     <t>Nguyễn Thị Linh Nhi</t>
@@ -49,7 +52,10 @@
     <t>13.png</t>
   </si>
   <si>
-    <t>HS0009</t>
+    <t>0987456321</t>
+  </si>
+  <si>
+    <t>HS0051</t>
   </si>
   <si>
     <t>Nguyễn Trần Văn Thuận</t>
@@ -64,7 +70,10 @@
     <t>14.png</t>
   </si>
   <si>
-    <t>HS0010</t>
+    <t>0874512369</t>
+  </si>
+  <si>
+    <t>HS0052</t>
   </si>
   <si>
     <t>Hoàng Tân Đại</t>
@@ -79,13 +88,19 @@
     <t>15.png</t>
   </si>
   <si>
-    <t>HS0011</t>
+    <t>0321485697</t>
+  </si>
+  <si>
+    <t>HS0053</t>
   </si>
   <si>
     <t>Trương Hoàng Giang</t>
   </si>
   <si>
     <t>16.png</t>
+  </si>
+  <si>
+    <t>0254136987</t>
   </si>
 </sst>
 </file>
@@ -93,10 +108,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="21">
@@ -116,6 +131,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -125,36 +155,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,23 +216,52 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,29 +269,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,19 +284,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,163 +410,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,17 +493,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,15 +517,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -532,11 +532,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -558,15 +582,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -580,162 +595,168 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1057,13 +1078,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="12.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="21.6666666666667" customWidth="1"/>
@@ -1071,9 +1092,10 @@
     <col min="4" max="4" width="12.2190476190476" customWidth="1"/>
     <col min="5" max="5" width="19.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="23.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="15.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1095,91 +1117,106 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3">
         <v>37238</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
         <v>37165</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
         <v>37101</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3">
         <v>37101</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>